<commit_message>
added good datasets; updated spreadsheet
</commit_message>
<xml_diff>
--- a/docs/ml-research/ml-research.xlsx
+++ b/docs/ml-research/ml-research.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landen/Desktop/Classes/Fall23/eecs581/park-sense/docs/ml-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3914CB7-7039-CA4D-A9FE-BA9B5EE53354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD00AA8-31C5-7B4E-AE50-0BA97468374A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1000" windowWidth="26900" windowHeight="16440" xr2:uid="{A662E122-3890-2044-A84F-9393FC5409CD}"/>
+    <workbookView xWindow="1520" yWindow="560" windowWidth="26900" windowHeight="16440" xr2:uid="{A662E122-3890-2044-A84F-9393FC5409CD}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="convolutions" sheetId="2" r:id="rId2"/>
+    <sheet name="parameters" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Data Requirements</t>
   </si>
@@ -113,6 +115,24 @@
   </si>
   <si>
     <t>Link/Location</t>
+  </si>
+  <si>
+    <t>Stanford Cars Dataset</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/datasets/jessicali9530/stanford-cars-dataset</t>
+  </si>
+  <si>
+    <t>Vehicle Detection Image Set</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/datasets/brsdincer/vehicle-detection-image-set</t>
+  </si>
+  <si>
+    <t>Binary, Decent Variation in orientation</t>
+  </si>
+  <si>
+    <t>Multi-class, more data</t>
   </si>
 </sst>
 </file>
@@ -174,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -209,6 +229,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,33 +547,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF7990C-3E5D-A145-8484-E99590845A94}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -559,7 +582,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -568,7 +591,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -577,7 +600,7 @@
       </c>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:3" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="101" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -586,26 +609,26 @@
       </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>2</v>
       </c>
@@ -616,10 +639,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>2</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -634,4 +680,28 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE5AE55-5270-C048-B22C-57E9867D5C2F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4D387D-10DC-114D-9C77-082C35C67151}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finalized sprint 1 research
</commit_message>
<xml_diff>
--- a/docs/ml-research/ml-research.xlsx
+++ b/docs/ml-research/ml-research.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landen/Desktop/Classes/Fall23/eecs581/park-sense/docs/ml-research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sepehrnoori/Desktop/School/Fall 2023/EECS 581/ParkSense/docs/ml-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD00AA8-31C5-7B4E-AE50-0BA97468374A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3BE480-6AAE-B943-AC51-0148DB6D3826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="560" windowWidth="26900" windowHeight="16440" xr2:uid="{A662E122-3890-2044-A84F-9393FC5409CD}"/>
+    <workbookView xWindow="1520" yWindow="500" windowWidth="26900" windowHeight="16340" activeTab="1" xr2:uid="{A662E122-3890-2044-A84F-9393FC5409CD}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Data Requirements</t>
   </si>
@@ -133,6 +133,75 @@
   </si>
   <si>
     <t>Multi-class, more data</t>
+  </si>
+  <si>
+    <t>Planned Parameters</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Loss function</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Reasoning</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>binary_crossentropy</t>
+  </si>
+  <si>
+    <t>We plan to use this loss function because it was designed for binary classification which is what ParkSense aims to do, whether an image contains a vehicle or not.</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>15-30</t>
+  </si>
+  <si>
+    <t>Activation function</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>Because sigmoid places the data between 0 and 1 which is a binary classification.</t>
+  </si>
+  <si>
+    <t>This coincides with previous binary classification models that we have developed similar to this model.</t>
+  </si>
+  <si>
+    <t>Number of Layers</t>
+  </si>
+  <si>
+    <t>Parameter Value</t>
+  </si>
+  <si>
+    <t>15-50</t>
+  </si>
+  <si>
+    <t>This is a educated guess since we don't really know what the optimal number of layers is going to be, especially when the model is running on a microcontroller. The thought process is that we want to keep the model as small as possible to decrease the amount of memory required to operate it.</t>
+  </si>
+  <si>
+    <t>Tends to be a very good fit for many machine learning applications. Expecting to try this out first and find out how well it will work for our project. The optimizer will also take a parameter of learning rate which will be modified to find the optimal learning rate for this use case.</t>
+  </si>
+  <si>
+    <t>Convolution Type</t>
+  </si>
+  <si>
+    <t>Conv2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on our research, most object classification models use Conv2D with ReLU for filtering and MaxPooling for condensing the image. </t>
+  </si>
+  <si>
+    <t>After completing our research we find that it may be simpler and more effective if we use a pretrained model and transfer learning to implement our model. However, since we are hoping to learn how to implement such a model from scratch, we will do so and compare our results with a pretrained model.</t>
   </si>
 </sst>
 </file>
@@ -182,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -190,48 +259,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -549,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF7990C-3E5D-A145-8484-E99590845A94}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,82 +669,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:4" ht="101" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -643,10 +752,10 @@
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
@@ -654,13 +763,13 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D12" t="s">
@@ -684,24 +793,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE5AE55-5270-C048-B22C-57E9867D5C2F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4D387D-10DC-114D-9C77-082C35C67151}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="3" width="58.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>